<commit_message>
EPBDS-12251 Smart Lookup Horizontal condition is matched incorrectly if the column contains empty values
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11727_Titled_HC_1.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11727_Titled_HC_1.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\incorrect_condition_match1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD747FC-157A-4486-876C-28F63C6411C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A384C2-EBDE-4A95-9E49-EFD77E8D9694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7840" yWindow="2160" windowWidth="28800" windowHeight="15560" xr2:uid="{B6CFAC92-A50A-4ED7-9D78-780E71329F6C}"/>
+    <workbookView xWindow="8480" yWindow="1740" windowWidth="23000" windowHeight="17540" xr2:uid="{B6CFAC92-A50A-4ED7-9D78-780E71329F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="36">
   <si>
     <t xml:space="preserve"> coverageType</t>
   </si>
@@ -220,10 +220,10 @@
     </r>
   </si>
   <si>
-    <t>Test BaseRateObj2BaseRateObjTest2</t>
-  </si>
-  <si>
     <t>Test BaseRateObj2 BaseRateObjTest2</t>
+  </si>
+  <si>
+    <t>/genderOrSpouse</t>
   </si>
 </sst>
 </file>
@@ -237,7 +237,7 @@
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -414,9 +414,9 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -447,12 +447,21 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -468,20 +477,11 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Comma 2 2" xfId="2" xr:uid="{13EAD83A-2F0C-45C7-B584-2B6F2E3941F0}"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{0796624E-0A1A-4DC9-B741-65077A426E3D}"/>
-    <cellStyle name="Comma 2 2" xfId="2" xr:uid="{13EAD83A-2F0C-45C7-B584-2B6F2E3941F0}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -795,62 +795,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4591F0F3-33F6-4EB8-B292-A657C0CEA6C4}">
   <dimension ref="B4:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="29.08984375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.90625" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="36.81640625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="55.1796875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="18.453125" collapsed="true"/>
+    <col min="3" max="3" width="29.08984375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.90625" customWidth="1"/>
+    <col min="10" max="10" width="36.81640625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="55.1796875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.453125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="2:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="17" t="s">
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="18"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="13"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="14" t="b">
+      <c r="D6" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="14" t="b">
+      <c r="E6" s="19"/>
+      <c r="F6" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="19"/>
       <c r="H6" s="2" t="b">
         <v>0</v>
       </c>
@@ -859,7 +859,7 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B7" s="13"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
@@ -883,10 +883,10 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B8" s="20">
+      <c r="B8" s="15">
         <v>0</v>
       </c>
-      <c r="C8" s="21"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="6">
         <v>0.01</v>
       </c>
@@ -907,10 +907,10 @@
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B9" s="20">
+      <c r="B9" s="15">
         <v>15</v>
       </c>
-      <c r="C9" s="21"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="8">
         <v>0.02</v>
       </c>
@@ -949,12 +949,12 @@
       <c r="I17" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C18" s="7" t="s">
@@ -1112,48 +1112,48 @@
       </c>
     </row>
     <row r="42" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="12"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
     </row>
     <row r="43" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="14" t="s">
         <v>18</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E43" s="14" t="s">
+      <c r="E43" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="16"/>
-      <c r="I43" s="17" t="s">
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="J43" s="18"/>
+      <c r="J43" s="21"/>
     </row>
     <row r="44" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C44" s="13"/>
+      <c r="C44" s="14"/>
       <c r="D44" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E44" s="14" t="b">
+      <c r="E44" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="F44" s="16"/>
-      <c r="G44" s="14" t="b">
+      <c r="F44" s="19"/>
+      <c r="G44" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="H44" s="16"/>
+      <c r="H44" s="19"/>
       <c r="I44" s="2" t="b">
         <v>0</v>
       </c>
@@ -1162,9 +1162,9 @@
       </c>
     </row>
     <row r="45" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C45" s="13"/>
+      <c r="C45" s="14"/>
       <c r="D45" s="5" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>4</v>
@@ -1235,7 +1235,7 @@
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.35">
@@ -1299,6 +1299,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C42:J42"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="E43:H43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
     <mergeCell ref="J17:M17"/>
     <mergeCell ref="B4:I4"/>
     <mergeCell ref="B5:B7"/>
@@ -1308,12 +1314,6 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C42:J42"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="E43:H43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EPBDS-12385 Smart Lookup Horizontal condition is matched incorrectly with the input data, if the columns are merged
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11727_Titled_HC_1.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11727_Titled_HC_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A384C2-EBDE-4A95-9E49-EFD77E8D9694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6D1151-D172-4E58-A934-5D7AE669848D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8480" yWindow="1740" windowWidth="23000" windowHeight="17540" xr2:uid="{B6CFAC92-A50A-4ED7-9D78-780E71329F6C}"/>
+    <workbookView xWindow="11870" yWindow="3390" windowWidth="24610" windowHeight="15030" xr2:uid="{B6CFAC92-A50A-4ED7-9D78-780E71329F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -447,35 +447,35 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -796,7 +796,7 @@
   <dimension ref="B4:M59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B5" sqref="B5:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -809,48 +809,48 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
     </row>
     <row r="5" spans="2:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="20" t="s">
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="21"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="14"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="17" t="b">
+      <c r="D6" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="17" t="b">
+      <c r="E6" s="16"/>
+      <c r="F6" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="G6" s="19"/>
+      <c r="G6" s="16"/>
       <c r="H6" s="2" t="b">
         <v>0</v>
       </c>
@@ -859,9 +859,9 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B7" s="14"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="5" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>4</v>
@@ -883,10 +883,10 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B8" s="15">
+      <c r="B8" s="20">
         <v>0</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="6">
         <v>0.01</v>
       </c>
@@ -907,10 +907,10 @@
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B9" s="15">
+      <c r="B9" s="20">
         <v>15</v>
       </c>
-      <c r="C9" s="16"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="8">
         <v>0.02</v>
       </c>
@@ -949,12 +949,12 @@
       <c r="I17" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J17" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C18" s="7" t="s">
@@ -1112,48 +1112,48 @@
       </c>
     </row>
     <row r="42" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="13"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
     </row>
     <row r="43" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E43" s="17" t="s">
+      <c r="E43" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="20" t="s">
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="J43" s="21"/>
+      <c r="J43" s="18"/>
     </row>
     <row r="44" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C44" s="14"/>
+      <c r="C44" s="13"/>
       <c r="D44" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E44" s="17" t="b">
+      <c r="E44" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="F44" s="19"/>
-      <c r="G44" s="17" t="b">
+      <c r="F44" s="16"/>
+      <c r="G44" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="H44" s="19"/>
+      <c r="H44" s="16"/>
       <c r="I44" s="2" t="b">
         <v>0</v>
       </c>
@@ -1162,7 +1162,7 @@
       </c>
     </row>
     <row r="45" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C45" s="14"/>
+      <c r="C45" s="13"/>
       <c r="D45" s="5" t="s">
         <v>35</v>
       </c>
@@ -1299,12 +1299,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C42:J42"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="E43:H43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
     <mergeCell ref="J17:M17"/>
     <mergeCell ref="B4:I4"/>
     <mergeCell ref="B5:B7"/>
@@ -1314,6 +1308,12 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C42:J42"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="E43:H43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>